<commit_message>
Tidy up off the filter list and report
</commit_message>
<xml_diff>
--- a/documentation/volere_shells.xlsx
+++ b/documentation/volere_shells.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ThomasFranklin/Tweet-Classification/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDB2E6A-2DE5-7241-BFA7-89F28F2A3216}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC65ECF-38DE-9D41-B249-ECB6DD13C56A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="1460" windowWidth="24640" windowHeight="13960" xr2:uid="{B7C3B58B-1264-694A-A8D2-9BCEF10305EA}"/>
   </bookViews>
@@ -45,15 +45,9 @@
     <t>Description:</t>
   </si>
   <si>
-    <t>The pre-processor shall send the processed Tweet for classification</t>
-  </si>
-  <si>
     <t>Rationale:</t>
   </si>
   <si>
-    <t>To be able to send processed Tweets to the classifier to be assigned a label</t>
-  </si>
-  <si>
     <t>Originator:</t>
   </si>
   <si>
@@ -102,30 +96,12 @@
     <t>Non-Functional</t>
   </si>
   <si>
-    <t>The pre-processor shall be configurable if processing should occur</t>
-  </si>
-  <si>
-    <t>To be able to control if Tweets should receive processing</t>
-  </si>
-  <si>
-    <t>If processing is enabled then apply rules, if no processing is enabled then Tweet body will not be altered</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
     <t>FR.02</t>
   </si>
   <si>
-    <t>The pre-processor shall give details if it is running</t>
-  </si>
-  <si>
-    <t>To be able to check if the pre-processor is running</t>
-  </si>
-  <si>
-    <t>An endpoint which will provide the current status of the service</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -144,9 +120,6 @@
     <t>NF.02</t>
   </si>
   <si>
-    <t>The classifier shall make use of a two-stage classification process</t>
-  </si>
-  <si>
     <t>The system should use a verification classification to ensure the accuracy is as high as possible</t>
   </si>
   <si>
@@ -156,9 +129,6 @@
     <t>NF.03</t>
   </si>
   <si>
-    <t>The classifier shall accurately store the data to the database</t>
-  </si>
-  <si>
     <t>The system has to ensure consistency and reliability</t>
   </si>
   <si>
@@ -168,9 +138,6 @@
     <t>FR.04</t>
   </si>
   <si>
-    <t>The database shall be able to link back a Tweet to a particular user</t>
-  </si>
-  <si>
     <t>The system has to ensure traceability between Tweets and users to allow for the data to be presented correctly</t>
   </si>
   <si>
@@ -180,18 +147,12 @@
     <t>FR.05</t>
   </si>
   <si>
-    <t>The database shall be able to link back a Tweet to a particular hashtag</t>
-  </si>
-  <si>
     <t>The system has to ensure traceability between Tweets and hashtags to allow for the data to be presented correctly</t>
   </si>
   <si>
     <t>FR.06</t>
   </si>
   <si>
-    <t>The stream shall be configurable with the filter list</t>
-  </si>
-  <si>
     <t>The system has to ensure that it has control over what Tweets get streamed in to the service</t>
   </si>
   <si>
@@ -201,9 +162,6 @@
     <t>NF.04</t>
   </si>
   <si>
-    <t>The stream shall only add Tweets that are not a retweet to the Queue</t>
-  </si>
-  <si>
     <t>As Retweets are repeated Tweets, processing them more than once will be counterproductive</t>
   </si>
   <si>
@@ -213,9 +171,6 @@
     <t>NF.05</t>
   </si>
   <si>
-    <t>The stream shall reconnect upon error</t>
-  </si>
-  <si>
     <t>As the service should be constantly streaming Tweets, it is important that it reconnects if there is ever an error</t>
   </si>
   <si>
@@ -225,9 +180,6 @@
     <t>NF.06</t>
   </si>
   <si>
-    <t>The queue reader shall ensure that the message is valid from the queue</t>
-  </si>
-  <si>
     <t>To ensure that integrity of the system is kept, and the correct message is processed</t>
   </si>
   <si>
@@ -237,9 +189,6 @@
     <t>FR.07</t>
   </si>
   <si>
-    <t>The queue reader shall be able to report on successes/failures</t>
-  </si>
-  <si>
     <t>To monitor the performance of the system</t>
   </si>
   <si>
@@ -249,9 +198,6 @@
     <t>FR.08</t>
   </si>
   <si>
-    <t>The queue reader shall remove/discard any items that are not a Tweet object</t>
-  </si>
-  <si>
     <t>To ensure that only relevant information is processed and kept</t>
   </si>
   <si>
@@ -261,15 +207,9 @@
     <t>FR.09</t>
   </si>
   <si>
-    <t>The pre-processor shall only handle Tweet objects from the queue reader</t>
-  </si>
-  <si>
     <t>FR.10</t>
   </si>
   <si>
-    <t>The frontend shall be able to receive requests</t>
-  </si>
-  <si>
     <t>To ensure that users can connect to the service</t>
   </si>
   <si>
@@ -279,9 +219,6 @@
     <t>FR.11</t>
   </si>
   <si>
-    <t>The frontend shall be able to display status information when user navigates to homepage</t>
-  </si>
-  <si>
     <t>To ensure that users can see the status of the system</t>
   </si>
   <si>
@@ -291,18 +228,12 @@
     <t>NF.07</t>
   </si>
   <si>
-    <t>The frontend shall only display relevant information to the status of the system</t>
-  </si>
-  <si>
     <t>To ensure that users only information about the status that are relevant, and errors/exceptions should be kept private</t>
   </si>
   <si>
     <t>NF.08</t>
   </si>
   <si>
-    <t>The database shall be free from SQL injection attempts</t>
-  </si>
-  <si>
     <t>To ensure that the database and its data is secure</t>
   </si>
   <si>
@@ -312,9 +243,6 @@
     <t>NF.09</t>
   </si>
   <si>
-    <t>The API search shall be secure</t>
-  </si>
-  <si>
     <t>To ensure that a user does not maliciously try and retrieve data</t>
   </si>
   <si>
@@ -324,9 +252,6 @@
     <t>NF.10</t>
   </si>
   <si>
-    <t>The frontend and API shall return responses within 10 seconds</t>
-  </si>
-  <si>
     <t>To ensure that a user does not get bored waiting on a request</t>
   </si>
   <si>
@@ -339,9 +264,6 @@
     <t>17,18,19,20</t>
   </si>
   <si>
-    <t>The API should return responses in JSON format</t>
-  </si>
-  <si>
     <t>To ensure that the frontend can handle the response and display the information to the user</t>
   </si>
   <si>
@@ -366,9 +288,6 @@
     <t>10,11,12,13</t>
   </si>
   <si>
-    <t>The Frontend shall provide help through tooltips</t>
-  </si>
-  <si>
     <t>To ensure that the system is easy to use and informative</t>
   </si>
   <si>
@@ -381,9 +300,6 @@
     <t>11,12</t>
   </si>
   <si>
-    <t>The frontend shall allow users to report particular terms</t>
-  </si>
-  <si>
     <t>In case a Tweet that doesn't match the filters that needs to be added</t>
   </si>
   <si>
@@ -393,13 +309,97 @@
     <t>NF.12</t>
   </si>
   <si>
-    <t>The frontend shall be pleasing to the eye</t>
-  </si>
-  <si>
     <t>As the site is how users will interact, it should be pleasant to look at</t>
   </si>
   <si>
     <t>Use of design best practises and HCI considerations</t>
+  </si>
+  <si>
+    <t>The system shall assign a rumour or non-rumor label to a processed Tweet</t>
+  </si>
+  <si>
+    <t>To be able to assign a classification label to a particular Tweet after processing has been applied</t>
+  </si>
+  <si>
+    <t>The system shall be configurable to account for the needs of the system</t>
+  </si>
+  <si>
+    <t>To be able to control the systems services, and enable certain filters, processing techniques</t>
+  </si>
+  <si>
+    <t>Configuration files for each service which are deployed at run time</t>
+  </si>
+  <si>
+    <t>The system shall provide details on if it is running</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To be able to check if the services are operational </t>
+  </si>
+  <si>
+    <t>Various endpoints and checks to ensure services are functional</t>
+  </si>
+  <si>
+    <t>The system shall make use of a two-stage classification process</t>
+  </si>
+  <si>
+    <t>The system shall accurately store the data to the database</t>
+  </si>
+  <si>
+    <t>The system shall be able to link back a Tweet to a particular user</t>
+  </si>
+  <si>
+    <t>The system shall be able to link back a Tweet to a particular hashtag</t>
+  </si>
+  <si>
+    <t>The system shall be configurable with the filter list</t>
+  </si>
+  <si>
+    <t>The system shall only add Tweets that are not a retweet to the Queue</t>
+  </si>
+  <si>
+    <t>The system shall be robust enough to restart on failure</t>
+  </si>
+  <si>
+    <t>The system shall ensure that the message is valid from the queue</t>
+  </si>
+  <si>
+    <t>The system shall be able to report on successes/failures</t>
+  </si>
+  <si>
+    <t>The system shall remove/discard any items that are not a Tweet object</t>
+  </si>
+  <si>
+    <t>The system shall only handle Tweet objects from the queue reader</t>
+  </si>
+  <si>
+    <t>The system shall be able to receive user requests</t>
+  </si>
+  <si>
+    <t>The system shall be able to display status information when user navigates to homepage</t>
+  </si>
+  <si>
+    <t>The system shall only display relevant information to the status of the system</t>
+  </si>
+  <si>
+    <t>The system shall be free from SQL injection attempts</t>
+  </si>
+  <si>
+    <t>The system shall be secure</t>
+  </si>
+  <si>
+    <t>The system shall be able to respond to user requests within 15 seconds</t>
+  </si>
+  <si>
+    <t>The system shall return responses in JSON format</t>
+  </si>
+  <si>
+    <t>The system shall provide help to the users</t>
+  </si>
+  <si>
+    <t>The system shall allow users to report particular terms</t>
+  </si>
+  <si>
+    <t>The system shall be pleasing to the eye</t>
   </si>
 </sst>
 </file>
@@ -1121,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07C206C-6A49-8B48-91D8-FF7EBD55957B}">
   <dimension ref="A1:G404"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="B258" sqref="B258:F259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1168,7 +1168,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -1187,10 +1187,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -1209,10 +1209,10 @@
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -1222,10 +1222,10 @@
     </row>
     <row r="8" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -1244,14 +1244,14 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="8">
         <v>5</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="8">
@@ -1270,27 +1270,27 @@
     </row>
     <row r="12" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="28"/>
@@ -1300,10 +1300,10 @@
     </row>
     <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" s="28"/>
       <c r="D14" s="28"/>
@@ -1319,13 +1319,13 @@
         <v>0</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>4</v>
@@ -1349,7 +1349,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
@@ -1368,10 +1368,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
@@ -1390,10 +1390,10 @@
     </row>
     <row r="22" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
@@ -1403,10 +1403,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -1425,14 +1425,14 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B25" s="8">
         <v>3</v>
       </c>
       <c r="C25" s="20"/>
       <c r="D25" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="8">
@@ -1451,27 +1451,27 @@
     </row>
     <row r="27" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C28" s="28"/>
       <c r="D28" s="28"/>
@@ -1481,10 +1481,10 @@
     </row>
     <row r="29" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
@@ -1500,7 +1500,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>2</v>
@@ -1530,7 +1530,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
@@ -1549,10 +1549,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
@@ -1571,10 +1571,10 @@
     </row>
     <row r="37" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
@@ -1584,10 +1584,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
@@ -1606,14 +1606,14 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B40" s="8">
         <v>2</v>
       </c>
       <c r="C40" s="20"/>
       <c r="D40" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E40" s="10"/>
       <c r="F40" s="8">
@@ -1632,27 +1632,27 @@
     </row>
     <row r="42" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E42" s="26"/>
       <c r="F42" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G42" s="1"/>
     </row>
     <row r="43" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
@@ -1662,10 +1662,10 @@
     </row>
     <row r="44" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C44" s="28"/>
       <c r="D44" s="28"/>
@@ -1681,7 +1681,7 @@
         <v>0</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>2</v>
@@ -1711,7 +1711,7 @@
         <v>5</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
@@ -1730,10 +1730,10 @@
     </row>
     <row r="50" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
@@ -1752,10 +1752,10 @@
     </row>
     <row r="52" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="18"/>
@@ -1765,10 +1765,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
@@ -1787,14 +1787,14 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B55" s="8">
         <v>5</v>
       </c>
       <c r="C55" s="20"/>
       <c r="D55" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E55" s="10"/>
       <c r="F55" s="8">
@@ -1813,27 +1813,27 @@
     </row>
     <row r="57" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E57" s="26"/>
       <c r="F57" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G57" s="1"/>
     </row>
     <row r="58" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C58" s="28"/>
       <c r="D58" s="28"/>
@@ -1843,10 +1843,10 @@
     </row>
     <row r="59" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C59" s="28"/>
       <c r="D59" s="28"/>
@@ -1862,13 +1862,13 @@
         <v>0</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>4</v>
@@ -1892,7 +1892,7 @@
         <v>5</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
@@ -1911,10 +1911,10 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C65" s="12"/>
       <c r="D65" s="12"/>
@@ -1933,10 +1933,10 @@
     </row>
     <row r="67" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C67" s="18"/>
       <c r="D67" s="18"/>
@@ -1946,10 +1946,10 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
@@ -1968,14 +1968,14 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B70" s="8">
         <v>5</v>
       </c>
       <c r="C70" s="20"/>
       <c r="D70" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E70" s="10"/>
       <c r="F70" s="8">
@@ -1994,27 +1994,27 @@
     </row>
     <row r="72" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E72" s="26"/>
       <c r="F72" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G72" s="1"/>
     </row>
     <row r="73" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B73" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C73" s="28"/>
       <c r="D73" s="28"/>
@@ -2024,10 +2024,10 @@
     </row>
     <row r="74" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B74" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C74" s="28"/>
       <c r="D74" s="28"/>
@@ -2043,13 +2043,13 @@
         <v>0</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>4</v>
@@ -2073,7 +2073,7 @@
         <v>5</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
@@ -2114,10 +2114,10 @@
     </row>
     <row r="82" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C82" s="18"/>
       <c r="D82" s="18"/>
@@ -2127,10 +2127,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C83" s="12"/>
       <c r="D83" s="12"/>
@@ -2149,14 +2149,14 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B85" s="8">
         <v>5</v>
       </c>
       <c r="C85" s="20"/>
       <c r="D85" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E85" s="10"/>
       <c r="F85" s="8">
@@ -2175,27 +2175,27 @@
     </row>
     <row r="87" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E87" s="26"/>
       <c r="F87" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G87" s="1"/>
     </row>
     <row r="88" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B88" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C88" s="28"/>
       <c r="D88" s="28"/>
@@ -2205,10 +2205,10 @@
     </row>
     <row r="89" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B89" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C89" s="28"/>
       <c r="D89" s="28"/>
@@ -2224,7 +2224,7 @@
         <v>0</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>2</v>
@@ -2254,7 +2254,7 @@
         <v>5</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="C93" s="12"/>
       <c r="D93" s="12"/>
@@ -2273,10 +2273,10 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C95" s="12"/>
       <c r="D95" s="12"/>
@@ -2295,10 +2295,10 @@
     </row>
     <row r="97" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B97" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C97" s="18"/>
       <c r="D97" s="18"/>
@@ -2308,10 +2308,10 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C98" s="12"/>
       <c r="D98" s="12"/>
@@ -2330,14 +2330,14 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B100" s="8">
         <v>5</v>
       </c>
       <c r="C100" s="20"/>
       <c r="D100" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E100" s="10"/>
       <c r="F100" s="8">
@@ -2356,27 +2356,27 @@
     </row>
     <row r="102" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C102" s="5"/>
       <c r="D102" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E102" s="26"/>
       <c r="F102" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G102" s="1"/>
     </row>
     <row r="103" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B103" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C103" s="28"/>
       <c r="D103" s="28"/>
@@ -2386,10 +2386,10 @@
     </row>
     <row r="104" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B104" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
@@ -2405,7 +2405,7 @@
         <v>0</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>2</v>
@@ -2435,7 +2435,7 @@
         <v>5</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
       <c r="C108" s="12"/>
       <c r="D108" s="12"/>
@@ -2454,10 +2454,10 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C110" s="12"/>
       <c r="D110" s="12"/>
@@ -2476,10 +2476,10 @@
     </row>
     <row r="112" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B112" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C112" s="18"/>
       <c r="D112" s="18"/>
@@ -2489,10 +2489,10 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C113" s="12"/>
       <c r="D113" s="12"/>
@@ -2511,14 +2511,14 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B115" s="8">
         <v>5</v>
       </c>
       <c r="C115" s="20"/>
       <c r="D115" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E115" s="10"/>
       <c r="F115" s="8">
@@ -2537,27 +2537,27 @@
     </row>
     <row r="117" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C117" s="5"/>
       <c r="D117" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E117" s="26"/>
       <c r="F117" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G117" s="1"/>
     </row>
     <row r="118" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B118" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C118" s="28"/>
       <c r="D118" s="28"/>
@@ -2567,10 +2567,10 @@
     </row>
     <row r="119" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B119" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C119" s="28"/>
       <c r="D119" s="28"/>
@@ -2586,7 +2586,7 @@
         <v>0</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>2</v>
@@ -2616,7 +2616,7 @@
         <v>5</v>
       </c>
       <c r="B123" s="11" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C123" s="12"/>
       <c r="D123" s="12"/>
@@ -2635,10 +2635,10 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B125" s="11" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C125" s="12"/>
       <c r="D125" s="12"/>
@@ -2657,10 +2657,10 @@
     </row>
     <row r="127" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B127" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C127" s="18"/>
       <c r="D127" s="18"/>
@@ -2670,10 +2670,10 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B128" s="11" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C128" s="12"/>
       <c r="D128" s="12"/>
@@ -2692,14 +2692,14 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B130" s="8">
         <v>5</v>
       </c>
       <c r="C130" s="20"/>
       <c r="D130" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E130" s="10"/>
       <c r="F130" s="8">
@@ -2718,27 +2718,27 @@
     </row>
     <row r="132" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C132" s="5"/>
       <c r="D132" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E132" s="26"/>
       <c r="F132" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G132" s="1"/>
     </row>
     <row r="133" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B133" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C133" s="28"/>
       <c r="D133" s="28"/>
@@ -2748,10 +2748,10 @@
     </row>
     <row r="134" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B134" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C134" s="28"/>
       <c r="D134" s="28"/>
@@ -2767,13 +2767,13 @@
         <v>0</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C136" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E136" s="6" t="s">
         <v>4</v>
@@ -2797,7 +2797,7 @@
         <v>5</v>
       </c>
       <c r="B138" s="11" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="C138" s="12"/>
       <c r="D138" s="12"/>
@@ -2816,10 +2816,10 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C140" s="12"/>
       <c r="D140" s="12"/>
@@ -2838,10 +2838,10 @@
     </row>
     <row r="142" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B142" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C142" s="18"/>
       <c r="D142" s="18"/>
@@ -2851,10 +2851,10 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B143" s="11" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C143" s="12"/>
       <c r="D143" s="12"/>
@@ -2873,14 +2873,14 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B145" s="8">
         <v>5</v>
       </c>
       <c r="C145" s="20"/>
       <c r="D145" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E145" s="10"/>
       <c r="F145" s="8">
@@ -2899,27 +2899,27 @@
     </row>
     <row r="147" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C147" s="5"/>
       <c r="D147" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E147" s="26"/>
       <c r="F147" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G147" s="1"/>
     </row>
     <row r="148" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B148" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C148" s="28"/>
       <c r="D148" s="28"/>
@@ -2929,10 +2929,10 @@
     </row>
     <row r="149" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B149" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C149" s="28"/>
       <c r="D149" s="28"/>
@@ -2948,13 +2948,13 @@
         <v>0</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C151" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D151" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E151" s="6" t="s">
         <v>4</v>
@@ -2978,7 +2978,7 @@
         <v>5</v>
       </c>
       <c r="B153" s="11" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="C153" s="12"/>
       <c r="D153" s="12"/>
@@ -2997,10 +2997,10 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B155" s="11" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C155" s="12"/>
       <c r="D155" s="12"/>
@@ -3019,10 +3019,10 @@
     </row>
     <row r="157" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B157" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C157" s="18"/>
       <c r="D157" s="18"/>
@@ -3032,10 +3032,10 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B158" s="11" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C158" s="12"/>
       <c r="D158" s="12"/>
@@ -3054,14 +3054,14 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B160" s="8">
         <v>5</v>
       </c>
       <c r="C160" s="20"/>
       <c r="D160" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E160" s="10"/>
       <c r="F160" s="8">
@@ -3080,27 +3080,27 @@
     </row>
     <row r="162" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C162" s="5"/>
       <c r="D162" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E162" s="26"/>
       <c r="F162" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G162" s="1"/>
     </row>
     <row r="163" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B163" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C163" s="28"/>
       <c r="D163" s="28"/>
@@ -3110,10 +3110,10 @@
     </row>
     <row r="164" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B164" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C164" s="28"/>
       <c r="D164" s="28"/>
@@ -3129,13 +3129,13 @@
         <v>0</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C166" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E166" s="6" t="s">
         <v>4</v>
@@ -3159,7 +3159,7 @@
         <v>5</v>
       </c>
       <c r="B168" s="11" t="s">
-        <v>66</v>
+        <v>111</v>
       </c>
       <c r="C168" s="12"/>
       <c r="D168" s="12"/>
@@ -3178,10 +3178,10 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B170" s="11" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C170" s="12"/>
       <c r="D170" s="12"/>
@@ -3200,10 +3200,10 @@
     </row>
     <row r="172" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B172" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C172" s="18"/>
       <c r="D172" s="18"/>
@@ -3213,10 +3213,10 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B173" s="11" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C173" s="12"/>
       <c r="D173" s="12"/>
@@ -3235,14 +3235,14 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B175" s="8">
         <v>5</v>
       </c>
       <c r="C175" s="20"/>
       <c r="D175" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E175" s="10"/>
       <c r="F175" s="8">
@@ -3261,27 +3261,27 @@
     </row>
     <row r="177" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C177" s="5"/>
       <c r="D177" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E177" s="26"/>
       <c r="F177" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G177" s="1"/>
     </row>
     <row r="178" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B178" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C178" s="28"/>
       <c r="D178" s="28"/>
@@ -3291,10 +3291,10 @@
     </row>
     <row r="179" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B179" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C179" s="28"/>
       <c r="D179" s="28"/>
@@ -3310,7 +3310,7 @@
         <v>0</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C181" s="6" t="s">
         <v>2</v>
@@ -3340,7 +3340,7 @@
         <v>5</v>
       </c>
       <c r="B183" s="11" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="C183" s="12"/>
       <c r="D183" s="12"/>
@@ -3359,10 +3359,10 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B185" s="11" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C185" s="12"/>
       <c r="D185" s="12"/>
@@ -3381,10 +3381,10 @@
     </row>
     <row r="187" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B187" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C187" s="18"/>
       <c r="D187" s="18"/>
@@ -3394,10 +3394,10 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B188" s="11" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C188" s="12"/>
       <c r="D188" s="12"/>
@@ -3416,14 +3416,14 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B190" s="8">
         <v>2</v>
       </c>
       <c r="C190" s="20"/>
       <c r="D190" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E190" s="10"/>
       <c r="F190" s="8">
@@ -3442,27 +3442,27 @@
     </row>
     <row r="192" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C192" s="5"/>
       <c r="D192" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E192" s="26"/>
       <c r="F192" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G192" s="1"/>
     </row>
     <row r="193" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B193" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C193" s="28"/>
       <c r="D193" s="28"/>
@@ -3472,10 +3472,10 @@
     </row>
     <row r="194" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B194" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C194" s="28"/>
       <c r="D194" s="28"/>
@@ -3491,7 +3491,7 @@
         <v>0</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C196" s="6" t="s">
         <v>2</v>
@@ -3521,7 +3521,7 @@
         <v>5</v>
       </c>
       <c r="B198" s="11" t="s">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="C198" s="12"/>
       <c r="D198" s="12"/>
@@ -3540,10 +3540,10 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B200" s="11" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C200" s="12"/>
       <c r="D200" s="12"/>
@@ -3562,10 +3562,10 @@
     </row>
     <row r="202" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B202" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C202" s="18"/>
       <c r="D202" s="18"/>
@@ -3575,10 +3575,10 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B203" s="11" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C203" s="12"/>
       <c r="D203" s="12"/>
@@ -3597,14 +3597,14 @@
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B205" s="8">
         <v>2</v>
       </c>
       <c r="C205" s="20"/>
       <c r="D205" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E205" s="10"/>
       <c r="F205" s="8">
@@ -3623,27 +3623,27 @@
     </row>
     <row r="207" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C207" s="5"/>
       <c r="D207" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E207" s="26"/>
       <c r="F207" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G207" s="1"/>
     </row>
     <row r="208" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B208" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C208" s="28"/>
       <c r="D208" s="28"/>
@@ -3653,10 +3653,10 @@
     </row>
     <row r="209" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B209" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C209" s="28"/>
       <c r="D209" s="28"/>
@@ -3672,7 +3672,7 @@
         <v>0</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="C211" s="6" t="s">
         <v>2</v>
@@ -3702,7 +3702,7 @@
         <v>5</v>
       </c>
       <c r="B213" s="11" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="C213" s="12"/>
       <c r="D213" s="12"/>
@@ -3721,10 +3721,10 @@
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B215" s="11" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C215" s="12"/>
       <c r="D215" s="12"/>
@@ -3743,10 +3743,10 @@
     </row>
     <row r="217" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B217" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C217" s="18"/>
       <c r="D217" s="18"/>
@@ -3756,10 +3756,10 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B218" s="11" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C218" s="12"/>
       <c r="D218" s="12"/>
@@ -3778,14 +3778,14 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B220" s="8">
         <v>2</v>
       </c>
       <c r="C220" s="20"/>
       <c r="D220" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E220" s="10"/>
       <c r="F220" s="8">
@@ -3804,27 +3804,27 @@
     </row>
     <row r="222" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C222" s="5"/>
       <c r="D222" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E222" s="26"/>
       <c r="F222" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G222" s="1"/>
     </row>
     <row r="223" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B223" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C223" s="28"/>
       <c r="D223" s="28"/>
@@ -3834,10 +3834,10 @@
     </row>
     <row r="224" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B224" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C224" s="28"/>
       <c r="D224" s="28"/>
@@ -3853,7 +3853,7 @@
         <v>0</v>
       </c>
       <c r="B226" s="8" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="C226" s="6" t="s">
         <v>2</v>
@@ -3883,7 +3883,7 @@
         <v>5</v>
       </c>
       <c r="B228" s="11" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="C228" s="12"/>
       <c r="D228" s="12"/>
@@ -3902,10 +3902,10 @@
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B230" s="11" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C230" s="12"/>
       <c r="D230" s="12"/>
@@ -3924,10 +3924,10 @@
     </row>
     <row r="232" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B232" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C232" s="18"/>
       <c r="D232" s="18"/>
@@ -3937,10 +3937,10 @@
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B233" s="11" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C233" s="12"/>
       <c r="D233" s="12"/>
@@ -3959,14 +3959,14 @@
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B235" s="8">
         <v>2</v>
       </c>
       <c r="C235" s="20"/>
       <c r="D235" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E235" s="10"/>
       <c r="F235" s="8">
@@ -3985,27 +3985,27 @@
     </row>
     <row r="237" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B237" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C237" s="5"/>
       <c r="D237" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E237" s="26"/>
       <c r="F237" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G237" s="1"/>
     </row>
     <row r="238" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B238" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C238" s="28"/>
       <c r="D238" s="28"/>
@@ -4015,10 +4015,10 @@
     </row>
     <row r="239" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B239" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C239" s="28"/>
       <c r="D239" s="28"/>
@@ -4034,7 +4034,7 @@
         <v>0</v>
       </c>
       <c r="B241" s="8" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C241" s="6" t="s">
         <v>2</v>
@@ -4064,7 +4064,7 @@
         <v>5</v>
       </c>
       <c r="B243" s="11" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="C243" s="12"/>
       <c r="D243" s="12"/>
@@ -4083,10 +4083,10 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B245" s="11" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="C245" s="12"/>
       <c r="D245" s="12"/>
@@ -4105,10 +4105,10 @@
     </row>
     <row r="247" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B247" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C247" s="18"/>
       <c r="D247" s="18"/>
@@ -4118,10 +4118,10 @@
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B248" s="11" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="C248" s="12"/>
       <c r="D248" s="12"/>
@@ -4140,14 +4140,14 @@
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B250" s="8">
         <v>5</v>
       </c>
       <c r="C250" s="20"/>
       <c r="D250" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E250" s="10"/>
       <c r="F250" s="8">
@@ -4166,27 +4166,27 @@
     </row>
     <row r="252" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C252" s="5"/>
       <c r="D252" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E252" s="26"/>
       <c r="F252" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G252" s="1"/>
     </row>
     <row r="253" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B253" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C253" s="28"/>
       <c r="D253" s="28"/>
@@ -4196,10 +4196,10 @@
     </row>
     <row r="254" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B254" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C254" s="28"/>
       <c r="D254" s="28"/>
@@ -4215,7 +4215,7 @@
         <v>0</v>
       </c>
       <c r="B256" s="8" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="C256" s="6" t="s">
         <v>2</v>
@@ -4245,7 +4245,7 @@
         <v>5</v>
       </c>
       <c r="B258" s="11" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="C258" s="12"/>
       <c r="D258" s="12"/>
@@ -4264,10 +4264,10 @@
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B260" s="11" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="C260" s="12"/>
       <c r="D260" s="12"/>
@@ -4286,10 +4286,10 @@
     </row>
     <row r="262" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B262" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C262" s="18"/>
       <c r="D262" s="18"/>
@@ -4299,10 +4299,10 @@
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B263" s="11" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C263" s="12"/>
       <c r="D263" s="12"/>
@@ -4321,14 +4321,14 @@
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A265" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B265" s="8">
         <v>5</v>
       </c>
       <c r="C265" s="20"/>
       <c r="D265" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E265" s="10"/>
       <c r="F265" s="8">
@@ -4347,27 +4347,27 @@
     </row>
     <row r="267" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B267" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C267" s="5"/>
       <c r="D267" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E267" s="26"/>
       <c r="F267" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G267" s="1"/>
     </row>
     <row r="268" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B268" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C268" s="28"/>
       <c r="D268" s="28"/>
@@ -4377,10 +4377,10 @@
     </row>
     <row r="269" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B269" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C269" s="28"/>
       <c r="D269" s="28"/>
@@ -4396,13 +4396,13 @@
         <v>0</v>
       </c>
       <c r="B271" s="8" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="C271" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D271" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E271" s="6" t="s">
         <v>4</v>
@@ -4426,7 +4426,7 @@
         <v>5</v>
       </c>
       <c r="B273" s="11" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="C273" s="12"/>
       <c r="D273" s="12"/>
@@ -4445,10 +4445,10 @@
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A275" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B275" s="11" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="C275" s="12"/>
       <c r="D275" s="12"/>
@@ -4467,10 +4467,10 @@
     </row>
     <row r="277" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B277" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C277" s="18"/>
       <c r="D277" s="18"/>
@@ -4480,10 +4480,10 @@
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A278" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B278" s="11" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C278" s="12"/>
       <c r="D278" s="12"/>
@@ -4502,14 +4502,14 @@
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A280" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B280" s="8">
         <v>5</v>
       </c>
       <c r="C280" s="20"/>
       <c r="D280" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E280" s="10"/>
       <c r="F280" s="8">
@@ -4528,27 +4528,27 @@
     </row>
     <row r="282" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B282" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C282" s="5"/>
       <c r="D282" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E282" s="26"/>
       <c r="F282" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G282" s="1"/>
     </row>
     <row r="283" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B283" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C283" s="28"/>
       <c r="D283" s="28"/>
@@ -4558,10 +4558,10 @@
     </row>
     <row r="284" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B284" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C284" s="28"/>
       <c r="D284" s="28"/>
@@ -4577,13 +4577,13 @@
         <v>0</v>
       </c>
       <c r="B286" s="8" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="C286" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D286" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E286" s="6" t="s">
         <v>4</v>
@@ -4607,7 +4607,7 @@
         <v>5</v>
       </c>
       <c r="B288" s="11" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="C288" s="12"/>
       <c r="D288" s="12"/>
@@ -4626,10 +4626,10 @@
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A290" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B290" s="11" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="C290" s="12"/>
       <c r="D290" s="12"/>
@@ -4648,10 +4648,10 @@
     </row>
     <row r="292" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B292" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C292" s="18"/>
       <c r="D292" s="18"/>
@@ -4661,10 +4661,10 @@
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A293" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B293" s="11" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="C293" s="12"/>
       <c r="D293" s="12"/>
@@ -4683,14 +4683,14 @@
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A295" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B295" s="8">
         <v>5</v>
       </c>
       <c r="C295" s="20"/>
       <c r="D295" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E295" s="10"/>
       <c r="F295" s="8">
@@ -4709,27 +4709,27 @@
     </row>
     <row r="297" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B297" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C297" s="5"/>
       <c r="D297" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E297" s="26"/>
       <c r="F297" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G297" s="1"/>
     </row>
     <row r="298" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B298" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C298" s="28"/>
       <c r="D298" s="28"/>
@@ -4739,10 +4739,10 @@
     </row>
     <row r="299" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B299" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C299" s="28"/>
       <c r="D299" s="28"/>
@@ -4758,13 +4758,13 @@
         <v>0</v>
       </c>
       <c r="B301" s="8" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="C301" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D301" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E301" s="6" t="s">
         <v>4</v>
@@ -4788,7 +4788,7 @@
         <v>5</v>
       </c>
       <c r="B303" s="11" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="C303" s="12"/>
       <c r="D303" s="12"/>
@@ -4807,10 +4807,10 @@
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A305" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B305" s="11" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="C305" s="12"/>
       <c r="D305" s="12"/>
@@ -4829,10 +4829,10 @@
     </row>
     <row r="307" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B307" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C307" s="18"/>
       <c r="D307" s="18"/>
@@ -4842,10 +4842,10 @@
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A308" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B308" s="11" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="C308" s="12"/>
       <c r="D308" s="12"/>
@@ -4864,14 +4864,14 @@
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A310" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B310" s="8">
         <v>5</v>
       </c>
       <c r="C310" s="20"/>
       <c r="D310" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E310" s="10"/>
       <c r="F310" s="8">
@@ -4890,27 +4890,27 @@
     </row>
     <row r="312" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B312" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C312" s="5"/>
       <c r="D312" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E312" s="26"/>
       <c r="F312" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G312" s="1"/>
     </row>
     <row r="313" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B313" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C313" s="28"/>
       <c r="D313" s="28"/>
@@ -4920,10 +4920,10 @@
     </row>
     <row r="314" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B314" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C314" s="28"/>
       <c r="D314" s="28"/>
@@ -4939,13 +4939,13 @@
         <v>0</v>
       </c>
       <c r="B316" s="8" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="C316" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D316" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E316" s="6" t="s">
         <v>4</v>
@@ -4969,7 +4969,7 @@
         <v>5</v>
       </c>
       <c r="B318" s="11" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="C318" s="12"/>
       <c r="D318" s="12"/>
@@ -4988,10 +4988,10 @@
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A320" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B320" s="11" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="C320" s="12"/>
       <c r="D320" s="12"/>
@@ -5010,10 +5010,10 @@
     </row>
     <row r="322" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B322" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C322" s="18"/>
       <c r="D322" s="18"/>
@@ -5023,10 +5023,10 @@
     </row>
     <row r="323" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A323" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B323" s="11" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="C323" s="12"/>
       <c r="D323" s="12"/>
@@ -5045,14 +5045,14 @@
     </row>
     <row r="325" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A325" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B325" s="8">
         <v>5</v>
       </c>
       <c r="C325" s="20"/>
       <c r="D325" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E325" s="10"/>
       <c r="F325" s="8">
@@ -5071,27 +5071,27 @@
     </row>
     <row r="327" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B327" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C327" s="5"/>
       <c r="D327" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E327" s="26"/>
       <c r="F327" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G327" s="1"/>
     </row>
     <row r="328" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B328" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C328" s="28"/>
       <c r="D328" s="28"/>
@@ -5101,10 +5101,10 @@
     </row>
     <row r="329" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B329" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C329" s="28"/>
       <c r="D329" s="28"/>
@@ -5120,7 +5120,7 @@
         <v>0</v>
       </c>
       <c r="B331" s="8" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="C331" s="6" t="s">
         <v>2</v>
@@ -5132,7 +5132,7 @@
         <v>4</v>
       </c>
       <c r="F331" s="8" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="G331" s="1"/>
     </row>
@@ -5150,7 +5150,7 @@
         <v>5</v>
       </c>
       <c r="B333" s="11" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="C333" s="12"/>
       <c r="D333" s="12"/>
@@ -5169,10 +5169,10 @@
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A335" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B335" s="11" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="C335" s="12"/>
       <c r="D335" s="12"/>
@@ -5191,10 +5191,10 @@
     </row>
     <row r="337" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B337" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C337" s="18"/>
       <c r="D337" s="18"/>
@@ -5204,10 +5204,10 @@
     </row>
     <row r="338" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A338" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B338" s="11" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="C338" s="12"/>
       <c r="D338" s="12"/>
@@ -5226,14 +5226,14 @@
     </row>
     <row r="340" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A340" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B340" s="8">
         <v>5</v>
       </c>
       <c r="C340" s="20"/>
       <c r="D340" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E340" s="10"/>
       <c r="F340" s="8">
@@ -5252,27 +5252,27 @@
     </row>
     <row r="342" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B342" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C342" s="5"/>
       <c r="D342" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E342" s="26"/>
       <c r="F342" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G342" s="1"/>
     </row>
     <row r="343" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B343" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C343" s="28"/>
       <c r="D343" s="28"/>
@@ -5282,10 +5282,10 @@
     </row>
     <row r="344" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B344" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C344" s="28"/>
       <c r="D344" s="28"/>
@@ -5301,13 +5301,13 @@
         <v>0</v>
       </c>
       <c r="B346" s="8" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="C346" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D346" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E346" s="6" t="s">
         <v>4</v>
@@ -5329,7 +5329,7 @@
         <v>5</v>
       </c>
       <c r="B348" s="11" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="C348" s="12"/>
       <c r="D348" s="12"/>
@@ -5346,10 +5346,10 @@
     </row>
     <row r="350" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A350" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B350" s="11" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="C350" s="12"/>
       <c r="D350" s="12"/>
@@ -5366,10 +5366,10 @@
     </row>
     <row r="352" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B352" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C352" s="18"/>
       <c r="D352" s="18"/>
@@ -5378,10 +5378,10 @@
     </row>
     <row r="353" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A353" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B353" s="11" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="C353" s="12"/>
       <c r="D353" s="12"/>
@@ -5398,14 +5398,14 @@
     </row>
     <row r="355" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A355" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B355" s="8">
         <v>5</v>
       </c>
       <c r="C355" s="20"/>
       <c r="D355" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E355" s="10"/>
       <c r="F355" s="8">
@@ -5422,26 +5422,26 @@
     </row>
     <row r="357" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B357" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C357" s="5"/>
       <c r="D357" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E357" s="26"/>
       <c r="F357" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="358" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B358" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C358" s="28"/>
       <c r="D358" s="28"/>
@@ -5450,10 +5450,10 @@
     </row>
     <row r="359" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B359" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C359" s="28"/>
       <c r="D359" s="28"/>
@@ -5466,7 +5466,7 @@
         <v>0</v>
       </c>
       <c r="B361" s="8" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="C361" s="6" t="s">
         <v>2</v>
@@ -5478,7 +5478,7 @@
         <v>4</v>
       </c>
       <c r="F361" s="8" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
     </row>
     <row r="362" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5494,7 +5494,7 @@
         <v>5</v>
       </c>
       <c r="B363" s="11" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="C363" s="12"/>
       <c r="D363" s="12"/>
@@ -5511,10 +5511,10 @@
     </row>
     <row r="365" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A365" s="34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B365" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="C365" s="12"/>
       <c r="D365" s="12"/>
@@ -5531,10 +5531,10 @@
     </row>
     <row r="367" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B367" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C367" s="18"/>
       <c r="D367" s="18"/>
@@ -5543,10 +5543,10 @@
     </row>
     <row r="368" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A368" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B368" s="11" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="C368" s="12"/>
       <c r="D368" s="12"/>
@@ -5563,14 +5563,14 @@
     </row>
     <row r="370" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A370" s="34" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B370" s="41">
         <v>5</v>
       </c>
       <c r="C370" s="43"/>
       <c r="D370" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E370" s="10"/>
       <c r="F370" s="41">
@@ -5587,26 +5587,26 @@
     </row>
     <row r="372" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B372" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C372" s="32"/>
       <c r="D372" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E372" s="45"/>
       <c r="F372" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="373" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B373" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C373" s="28"/>
       <c r="D373" s="28"/>
@@ -5615,10 +5615,10 @@
     </row>
     <row r="374" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B374" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C374" s="28"/>
       <c r="D374" s="28"/>
@@ -5631,7 +5631,7 @@
         <v>0</v>
       </c>
       <c r="B376" s="8" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="C376" s="6" t="s">
         <v>2</v>
@@ -5643,7 +5643,7 @@
         <v>4</v>
       </c>
       <c r="F376" s="8" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
     </row>
     <row r="377" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5659,7 +5659,7 @@
         <v>5</v>
       </c>
       <c r="B378" s="11" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C378" s="12"/>
       <c r="D378" s="12"/>
@@ -5676,10 +5676,10 @@
     </row>
     <row r="380" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A380" s="34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B380" s="11" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="C380" s="12"/>
       <c r="D380" s="12"/>
@@ -5696,10 +5696,10 @@
     </row>
     <row r="382" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B382" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C382" s="18"/>
       <c r="D382" s="18"/>
@@ -5708,10 +5708,10 @@
     </row>
     <row r="383" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A383" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B383" s="11" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="C383" s="12"/>
       <c r="D383" s="12"/>
@@ -5728,14 +5728,14 @@
     </row>
     <row r="385" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A385" s="34" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B385" s="41">
         <v>5</v>
       </c>
       <c r="C385" s="43"/>
       <c r="D385" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E385" s="10"/>
       <c r="F385" s="41">
@@ -5752,26 +5752,26 @@
     </row>
     <row r="387" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B387" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C387" s="32"/>
       <c r="D387" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E387" s="45"/>
       <c r="F387" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="388" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B388" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C388" s="28"/>
       <c r="D388" s="28"/>
@@ -5780,10 +5780,10 @@
     </row>
     <row r="389" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B389" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C389" s="28"/>
       <c r="D389" s="28"/>
@@ -5796,19 +5796,19 @@
         <v>0</v>
       </c>
       <c r="B391" s="8" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="C391" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D391" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E391" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F391" s="8" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
     </row>
     <row r="392" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5824,7 +5824,7 @@
         <v>5</v>
       </c>
       <c r="B393" s="11" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C393" s="12"/>
       <c r="D393" s="12"/>
@@ -5841,10 +5841,10 @@
     </row>
     <row r="395" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A395" s="34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B395" s="11" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="C395" s="12"/>
       <c r="D395" s="12"/>
@@ -5861,10 +5861,10 @@
     </row>
     <row r="397" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B397" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C397" s="18"/>
       <c r="D397" s="18"/>
@@ -5873,10 +5873,10 @@
     </row>
     <row r="398" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A398" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B398" s="11" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="C398" s="12"/>
       <c r="D398" s="12"/>
@@ -5893,14 +5893,14 @@
     </row>
     <row r="400" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A400" s="34" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B400" s="41">
         <v>5</v>
       </c>
       <c r="C400" s="43"/>
       <c r="D400" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E400" s="10"/>
       <c r="F400" s="41">
@@ -5917,26 +5917,26 @@
     </row>
     <row r="402" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A402" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B402" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C402" s="32"/>
       <c r="D402" s="25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E402" s="45"/>
       <c r="F402" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="403" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B403" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C403" s="28"/>
       <c r="D403" s="28"/>
@@ -5945,10 +5945,10 @@
     </row>
     <row r="404" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B404" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C404" s="28"/>
       <c r="D404" s="28"/>

</xml_diff>

<commit_message>
Additional work on tooltips and report
</commit_message>
<xml_diff>
--- a/documentation/volere_shells.xlsx
+++ b/documentation/volere_shells.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ThomasFranklin/Tweet-Classification/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC65ECF-38DE-9D41-B249-ECB6DD13C56A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B199940-9F2A-004E-BA93-8542791406FD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="1460" windowWidth="24640" windowHeight="13960" xr2:uid="{B7C3B58B-1264-694A-A8D2-9BCEF10305EA}"/>
   </bookViews>
@@ -1121,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07C206C-6A49-8B48-91D8-FF7EBD55957B}">
   <dimension ref="A1:G404"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="B258" sqref="B258:F259"/>
+    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
+      <selection activeCell="B378" sqref="B378:F379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>